<commit_message>
Et bim ! Tout les mails c'est bon ! ( à re tester quand même ;)
</commit_message>
<xml_diff>
--- a/src/Stolons/wwwroot/bills/Consumer/2/2016_20_2.xlsx
+++ b/src/Stolons/wwwroot/bills/Consumer/2/2016_20_2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Association Stolons</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Edité le :</t>
   </si>
   <si>
-    <t>19/05/2016 14:40:42</t>
+    <t>19/05/2016 17:26:29</t>
   </si>
   <si>
     <t>Produits de votre panier de la semaine</t>
@@ -74,22 +74,31 @@
     <t>MONTANT</t>
   </si>
   <si>
+    <t>Pain complet</t>
+  </si>
+  <si>
+    <t>Pains</t>
+  </si>
+  <si>
+    <t>A la pièce</t>
+  </si>
+  <si>
+    <t>Tomates grappe</t>
+  </si>
+  <si>
+    <t>Légumes</t>
+  </si>
+  <si>
+    <t>Au poids</t>
+  </si>
+  <si>
+    <t>Radis</t>
+  </si>
+  <si>
+    <t>Salade</t>
+  </si>
+  <si>
     <t>Pomme de terre</t>
-  </si>
-  <si>
-    <t>Légumes</t>
-  </si>
-  <si>
-    <t>Au poids</t>
-  </si>
-  <si>
-    <t>Salade</t>
-  </si>
-  <si>
-    <t>A la pièce</t>
-  </si>
-  <si>
-    <t>Radis</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL : </t>
@@ -231,7 +240,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0" view="pageLayout"/>
   </sheetViews>
@@ -386,10 +395,10 @@
         <v>22</v>
       </c>
       <c r="D16" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="12">
         <f>D16*E16</f>
@@ -400,52 +409,92 @@
         <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="12">
         <f>D17*E17</f>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4</v>
+      </c>
+      <c r="E18" s="0">
+        <v>2</v>
+      </c>
+      <c r="F18" s="12">
+        <f>D18*E18</f>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0">
+        <v>2</v>
+      </c>
+      <c r="F19" s="12">
+        <f>D19*E19</f>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="7">
-        <v>4</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="13">
-        <f>D18*E18</f>
-      </c>
-    </row>
-    <row r="19">
-      <c r="E19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="14">
-        <f>SUBTOTAL(9,F7:F18)</f>
+      <c r="D20" s="7">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>3</v>
+      </c>
+      <c r="F20" s="13">
+        <f>D20*E20</f>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="14">
+        <f>SUBTOTAL(9,F7:F20)</f>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>